<commit_message>
Update CT parameters - compute kd = koc * foc (close #123, close #105)
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitatdevalencia-my.sharepoint.com/personal/pablo_amador_uv_es/Documents/ERAHUMED_SHINY/rice_mod/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{03EC5619-D1AC-4B06-88D2-39B3F75C9311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70F45982-DF8B-467D-ADDC-F295354EB4A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CDA821-3CD5-46F1-BEDE-7D9C54A3D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>chemical</t>
   </si>
@@ -206,13 +206,16 @@
   </si>
   <si>
     <t>Active sediment layer depth (m)</t>
+  </si>
+  <si>
+    <t>koc_cm3_g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,8 +247,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,10 +270,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -294,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,8 +323,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -638,524 +665,536 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A82EF9-D59D-445F-8AC5-80173FC1E833}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="7.44140625" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.44140625" customWidth="1"/>
-    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.44140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.44140625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" style="8"/>
+    <col min="21" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="R1" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
         <v>0.2</v>
       </c>
-      <c r="D2">
-        <v>5.8</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="7">
         <v>0.11002336199364211</v>
       </c>
-      <c r="F2">
+      <c r="E2" s="7">
         <v>0.23104906018664842</v>
       </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2">
+      <c r="F2" s="7">
+        <v>20</v>
+      </c>
+      <c r="G2" s="7">
         <v>0.23104906018664842</v>
       </c>
-      <c r="I2">
-        <v>20</v>
-      </c>
-      <c r="J2">
+      <c r="H2" s="7">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7">
         <v>2</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="M2">
-        <v>20</v>
-      </c>
-      <c r="N2">
+      <c r="L2" s="7">
+        <v>20</v>
+      </c>
+      <c r="M2" s="7">
         <v>222.67699999999999</v>
       </c>
-      <c r="O2">
-        <v>2.58</v>
-      </c>
-      <c r="P2">
-        <v>2.58</v>
-      </c>
-      <c r="Q2">
-        <v>2.58</v>
-      </c>
-      <c r="R2" s="5">
-        <v>29503</v>
+      <c r="N2" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O2" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P2" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>2950</v>
+      </c>
+      <c r="R2" s="7">
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
         <v>0.2</v>
       </c>
-      <c r="D3">
-        <v>208.22399999999999</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="7">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="F3">
+      <c r="E3" s="7">
         <v>0.20799999999999999</v>
       </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3">
+      <c r="F3" s="7">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I3">
-        <v>20</v>
-      </c>
-      <c r="J3">
+      <c r="H3" s="7">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7">
         <v>2</v>
       </c>
-      <c r="K3">
+      <c r="J3" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L3" s="5">
+      <c r="K3" s="7">
         <v>0.114</v>
       </c>
-      <c r="M3">
-        <v>20</v>
-      </c>
-      <c r="N3">
+      <c r="L3" s="7">
+        <v>20</v>
+      </c>
+      <c r="M3" s="7">
         <v>403.33800000000002</v>
       </c>
-      <c r="O3">
-        <v>2.58</v>
-      </c>
-      <c r="P3">
-        <v>2.58</v>
-      </c>
-      <c r="Q3">
-        <v>2.58</v>
-      </c>
-      <c r="R3">
-        <v>6.73</v>
+      <c r="N3" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O3" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P3" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="R3" s="8">
+        <v>589</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
         <v>0.2</v>
       </c>
-      <c r="D4">
-        <v>1.63</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="7">
         <v>0.46200000000000002</v>
       </c>
-      <c r="F4">
+      <c r="E4" s="7">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-      <c r="H4">
+      <c r="F4" s="7">
+        <v>20</v>
+      </c>
+      <c r="G4" s="7">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="I4">
-        <v>20</v>
-      </c>
-      <c r="J4">
+      <c r="H4" s="7">
+        <v>20</v>
+      </c>
+      <c r="I4" s="7">
         <v>2</v>
       </c>
-      <c r="K4">
+      <c r="J4" s="7">
         <v>0.01</v>
       </c>
-      <c r="L4">
+      <c r="K4" s="7">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="M4">
-        <v>20</v>
-      </c>
-      <c r="N4">
+      <c r="L4" s="7">
+        <v>20</v>
+      </c>
+      <c r="M4" s="7">
         <v>240.28</v>
       </c>
-      <c r="O4">
-        <v>2.58</v>
-      </c>
-      <c r="P4">
-        <v>2.58</v>
-      </c>
-      <c r="Q4">
-        <v>2.58</v>
-      </c>
-      <c r="R4" s="5">
-        <v>71123</v>
+      <c r="N4" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O4" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P4" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>7112</v>
+      </c>
+      <c r="R4" s="8">
+        <v>55.3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
         <v>0.2</v>
       </c>
-      <c r="D5">
-        <v>2.1</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="7">
         <v>0.24755256448569476</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="7">
         <v>3.0136833937388925E-2</v>
       </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
+      <c r="F5" s="7">
+        <v>20</v>
+      </c>
+      <c r="G5" s="7">
         <v>0.11748257297626191</v>
       </c>
-      <c r="I5">
-        <v>20</v>
-      </c>
-      <c r="J5">
+      <c r="H5" s="7">
+        <v>20</v>
+      </c>
+      <c r="I5" s="7">
         <v>2</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
         <v>4.6209812037329684E-2</v>
       </c>
-      <c r="M5">
-        <v>20</v>
-      </c>
-      <c r="N5">
+      <c r="L5" s="7">
+        <v>20</v>
+      </c>
+      <c r="M5" s="7">
         <v>325.5</v>
       </c>
-      <c r="O5">
-        <v>2.58</v>
-      </c>
-      <c r="P5">
-        <v>2.58</v>
-      </c>
-      <c r="Q5">
-        <v>2.58</v>
-      </c>
-      <c r="R5">
+      <c r="N5" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O5" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P5" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>53</v>
+      </c>
+      <c r="R5" s="8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.161</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F6" s="7">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H6" s="7">
+        <v>20</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.126</v>
+      </c>
+      <c r="L6" s="7">
+        <v>20</v>
+      </c>
+      <c r="M6" s="7">
+        <v>357.38</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O6" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P6" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>0.44</v>
+      </c>
+      <c r="R6" s="8">
+        <v>5247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>9.4E-2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F7" s="7">
+        <v>20</v>
+      </c>
+      <c r="G7" s="7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H7" s="7">
+        <v>20</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="L7" s="7">
+        <v>20</v>
+      </c>
+      <c r="M7" s="7">
+        <v>406.3</v>
+      </c>
+      <c r="N7" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O7" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P7" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>15</v>
+      </c>
+      <c r="R7" s="7">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>20</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>20</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="L8" s="7">
+        <v>20</v>
+      </c>
+      <c r="M8" s="7">
+        <v>200.62</v>
+      </c>
+      <c r="N8" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O8" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P8" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>250000</v>
+      </c>
+      <c r="R8" s="8">
+        <v>73.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.248</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F9" s="7">
+        <v>20</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="H9" s="7">
+        <v>20</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L9" s="7">
+        <v>20</v>
+      </c>
+      <c r="M9" s="7">
+        <v>483.4</v>
+      </c>
+      <c r="N9" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="O9" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="P9" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="Q9" s="7">
         <v>408</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0.2</v>
-      </c>
-      <c r="D6">
-        <v>5.39</v>
-      </c>
-      <c r="E6">
-        <v>0.161</v>
-      </c>
-      <c r="F6">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I6">
-        <v>20</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0.126</v>
-      </c>
-      <c r="M6">
-        <v>20</v>
-      </c>
-      <c r="N6">
-        <v>357.38</v>
-      </c>
-      <c r="O6">
-        <v>2.58</v>
-      </c>
-      <c r="P6">
-        <v>2.58</v>
-      </c>
-      <c r="Q6">
-        <v>2.58</v>
-      </c>
-      <c r="R6" s="5">
-        <v>1803</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0.2</v>
-      </c>
-      <c r="D7">
-        <v>109.04</v>
-      </c>
-      <c r="E7">
-        <v>9.4E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
-      </c>
-      <c r="H7">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I7">
-        <v>20</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7">
-        <v>1E-3</v>
-      </c>
-      <c r="L7">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="M7">
-        <v>20</v>
-      </c>
-      <c r="N7">
-        <v>406.3</v>
-      </c>
-      <c r="O7">
-        <v>2.58</v>
-      </c>
-      <c r="P7">
-        <v>2.58</v>
-      </c>
-      <c r="Q7">
-        <v>2.58</v>
-      </c>
-      <c r="R7" s="5">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0.2</v>
-      </c>
-      <c r="D8">
-        <v>0.03</v>
-      </c>
-      <c r="E8">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="F8">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
-      <c r="H8">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="I8">
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="M8">
-        <v>20</v>
-      </c>
-      <c r="N8">
-        <v>200.62</v>
-      </c>
-      <c r="O8">
-        <v>2.58</v>
-      </c>
-      <c r="P8">
-        <v>2.58</v>
-      </c>
-      <c r="Q8">
-        <v>2.58</v>
-      </c>
-      <c r="R8" s="6">
-        <v>293903</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0.2</v>
-      </c>
-      <c r="D9">
-        <v>2.1</v>
-      </c>
-      <c r="E9">
-        <v>0.248</v>
-      </c>
-      <c r="F9">
-        <v>0.03</v>
-      </c>
-      <c r="G9">
-        <v>20</v>
-      </c>
-      <c r="H9">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="I9">
-        <v>20</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="M9">
-        <v>20</v>
-      </c>
-      <c r="N9">
-        <v>483.4</v>
-      </c>
-      <c r="O9">
-        <v>2.58</v>
-      </c>
-      <c r="P9">
-        <v>2.58</v>
-      </c>
-      <c r="Q9">
-        <v>2.58</v>
-      </c>
-      <c r="R9" s="5">
-        <v>4083</v>
+      <c r="R9" s="8">
+        <v>73.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ct_parameters.xlsx: add mock ssd_mu and ssd_sigma columns + remove cell formatting
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CDA821-3CD5-46F1-BEDE-7D9C54A3D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7595EF8D-68FF-4D4F-B273-126A52C5F444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
+    <workbookView xWindow="-28920" yWindow="-7230" windowWidth="29040" windowHeight="15720" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical Properties" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>chemical</t>
   </si>
@@ -209,13 +209,19 @@
   </si>
   <si>
     <t>koc_cm3_g</t>
+  </si>
+  <si>
+    <t>ssd_mu</t>
+  </si>
+  <si>
+    <t>ssd_sigma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,21 +253,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -273,11 +264,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -315,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -323,14 +309,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -667,534 +648,588 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A82EF9-D59D-445F-8AC5-80173FC1E833}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.44140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.44140625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.44140625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="8"/>
-    <col min="21" max="16384" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.44140625" style="5" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" style="6"/>
+    <col min="21" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="S1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>0.2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2">
         <v>0.11002336199364211</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2">
         <v>0.23104906018664842</v>
       </c>
-      <c r="F2" s="7">
-        <v>20</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
         <v>0.23104906018664842</v>
       </c>
-      <c r="H2" s="7">
-        <v>20</v>
-      </c>
-      <c r="I2" s="7">
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="J2" s="7">
-        <v>0</v>
-      </c>
-      <c r="K2" s="7">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="L2" s="7">
-        <v>20</v>
-      </c>
-      <c r="M2" s="7">
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
         <v>222.67699999999999</v>
       </c>
-      <c r="N2" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O2" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P2" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q2" s="7">
+      <c r="N2">
+        <v>2.58</v>
+      </c>
+      <c r="O2">
+        <v>2.58</v>
+      </c>
+      <c r="P2">
+        <v>2.58</v>
+      </c>
+      <c r="Q2">
         <v>2950</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>0.2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3">
         <v>0.20799999999999999</v>
       </c>
-      <c r="F3" s="7">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H3" s="7">
-        <v>20</v>
-      </c>
-      <c r="I3" s="7">
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3">
         <v>0.114</v>
       </c>
-      <c r="L3" s="7">
-        <v>20</v>
-      </c>
-      <c r="M3" s="7">
+      <c r="L3">
+        <v>20</v>
+      </c>
+      <c r="M3">
         <v>403.33800000000002</v>
       </c>
-      <c r="N3" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O3" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P3" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q3" s="7">
+      <c r="N3">
+        <v>2.58</v>
+      </c>
+      <c r="O3">
+        <v>2.58</v>
+      </c>
+      <c r="P3">
+        <v>2.58</v>
+      </c>
+      <c r="Q3">
         <v>6.7</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3">
         <v>589</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>0.2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4">
         <v>0.46200000000000002</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="F4" s="7">
-        <v>20</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="H4" s="7">
-        <v>20</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4">
         <v>0.01</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L4" s="7">
-        <v>20</v>
-      </c>
-      <c r="M4" s="7">
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
         <v>240.28</v>
       </c>
-      <c r="N4" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O4" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P4" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q4" s="7">
+      <c r="N4">
+        <v>2.58</v>
+      </c>
+      <c r="O4">
+        <v>2.58</v>
+      </c>
+      <c r="P4">
+        <v>2.58</v>
+      </c>
+      <c r="Q4">
         <v>7112</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4">
         <v>55.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>0.2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5">
         <v>0.24755256448569476</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5">
         <v>3.0136833937388925E-2</v>
       </c>
-      <c r="F5" s="7">
-        <v>20</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
         <v>0.11748257297626191</v>
       </c>
-      <c r="H5" s="7">
-        <v>20</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>4.6209812037329684E-2</v>
       </c>
-      <c r="L5" s="7">
-        <v>20</v>
-      </c>
-      <c r="M5" s="7">
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5">
         <v>325.5</v>
       </c>
-      <c r="N5" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O5" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P5" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q5" s="7">
+      <c r="N5">
+        <v>2.58</v>
+      </c>
+      <c r="O5">
+        <v>2.58</v>
+      </c>
+      <c r="P5">
+        <v>2.58</v>
+      </c>
+      <c r="Q5">
         <v>53</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>0.2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6">
         <v>0.161</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F6" s="7">
-        <v>20</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H6" s="7">
-        <v>20</v>
-      </c>
-      <c r="I6" s="7">
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>0.126</v>
       </c>
-      <c r="L6" s="7">
-        <v>20</v>
-      </c>
-      <c r="M6" s="7">
+      <c r="L6">
+        <v>20</v>
+      </c>
+      <c r="M6">
         <v>357.38</v>
       </c>
-      <c r="N6" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O6" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P6" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q6" s="7">
+      <c r="N6">
+        <v>2.58</v>
+      </c>
+      <c r="O6">
+        <v>2.58</v>
+      </c>
+      <c r="P6">
+        <v>2.58</v>
+      </c>
+      <c r="Q6">
         <v>0.44</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6">
         <v>5247</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>0.2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7">
         <v>9.4E-2</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7">
         <v>0.23100000000000001</v>
       </c>
-      <c r="F7" s="7">
-        <v>20</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H7" s="7">
-        <v>20</v>
-      </c>
-      <c r="I7" s="7">
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7">
         <v>2</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7">
         <v>1E-3</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7">
         <v>0.23100000000000001</v>
       </c>
-      <c r="L7" s="7">
-        <v>20</v>
-      </c>
-      <c r="M7" s="7">
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="M7">
         <v>406.3</v>
       </c>
-      <c r="N7" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O7" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P7" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q7" s="7">
+      <c r="N7">
+        <v>2.58</v>
+      </c>
+      <c r="O7">
+        <v>2.58</v>
+      </c>
+      <c r="P7">
+        <v>2.58</v>
+      </c>
+      <c r="Q7">
         <v>15</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7">
         <v>3200</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="7">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>0.2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8">
         <v>0.16500000000000001</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F8" s="7">
-        <v>20</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="G8">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="H8" s="7">
-        <v>20</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="L8" s="7">
-        <v>20</v>
-      </c>
-      <c r="M8" s="7">
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
         <v>200.62</v>
       </c>
-      <c r="N8" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O8" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P8" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q8" s="10">
+      <c r="N8">
+        <v>2.58</v>
+      </c>
+      <c r="O8">
+        <v>2.58</v>
+      </c>
+      <c r="P8">
+        <v>2.58</v>
+      </c>
+      <c r="Q8">
         <v>250000</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8">
         <v>73.88</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
         <v>0.2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9">
         <v>0.248</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9">
         <v>0.03</v>
       </c>
-      <c r="F9" s="7">
-        <v>20</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
         <v>0.11700000000000001</v>
       </c>
-      <c r="H9" s="7">
-        <v>20</v>
-      </c>
-      <c r="I9" s="7">
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9">
         <v>2</v>
       </c>
-      <c r="J9" s="7">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="L9" s="7">
-        <v>20</v>
-      </c>
-      <c r="M9" s="7">
+      <c r="L9">
+        <v>20</v>
+      </c>
+      <c r="M9">
         <v>483.4</v>
       </c>
-      <c r="N9" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="O9" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="P9" s="7">
-        <v>2.58</v>
-      </c>
-      <c r="Q9" s="7">
+      <c r="N9">
+        <v>2.58</v>
+      </c>
+      <c r="O9">
+        <v>2.58</v>
+      </c>
+      <c r="P9">
+        <v>2.58</v>
+      </c>
+      <c r="Q9">
         <v>408</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9">
         <v>73.2</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ct_parameters.xlsx raw data with TMoA
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7595EF8D-68FF-4D4F-B273-126A52C5F444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC712B1-5204-41DB-BC3E-D5C2EBE09781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-7230" windowWidth="29040" windowHeight="15720" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical Properties" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>chemical</t>
   </si>
@@ -215,13 +215,19 @@
   </si>
   <si>
     <t>ssd_sigma</t>
+  </si>
+  <si>
+    <t>tmoa</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +271,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -312,6 +325,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -646,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A82EF9-D59D-445F-8AC5-80173FC1E833}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,11 +685,11 @@
     <col min="17" max="17" width="8.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.44140625" style="5" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="6"/>
+    <col min="20" max="20" width="10.21875" style="6" customWidth="1"/>
     <col min="21" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -735,8 +750,11 @@
       <c r="T1" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U1" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -797,8 +815,11 @@
       <c r="T2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -859,8 +880,11 @@
       <c r="T3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -921,8 +945,11 @@
       <c r="T4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -983,8 +1010,11 @@
       <c r="T5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U5" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1045,8 +1075,11 @@
       <c r="T6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U6" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1107,8 +1140,11 @@
       <c r="T7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1169,8 +1205,11 @@
       <c r="T8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1230,6 +1269,9 @@
       </c>
       <c r="T9">
         <v>1</v>
+      </c>
+      <c r="U9" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add different parameters for acute and chronic risk SSD
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC712B1-5204-41DB-BC3E-D5C2EBE09781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB8AD16-6402-49EA-8211-B57215303034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>chemical</t>
   </si>
@@ -211,23 +211,29 @@
     <t>koc_cm3_g</t>
   </si>
   <si>
-    <t>ssd_mu</t>
-  </si>
-  <si>
-    <t>ssd_sigma</t>
-  </si>
-  <si>
     <t>tmoa</t>
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>ssd_acute_mu</t>
+  </si>
+  <si>
+    <t>ssd_acute_sigma</t>
+  </si>
+  <si>
+    <t>ssd_chronic_mu</t>
+  </si>
+  <si>
+    <t>ssd_chronic_sigma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +280,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -326,7 +340,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -661,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A82EF9-D59D-445F-8AC5-80173FC1E833}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +703,7 @@
     <col min="21" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -745,16 +759,22 @@
         <v>56</v>
       </c>
       <c r="S1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -815,11 +835,17 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="9">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -880,11 +906,17 @@
       <c r="T3">
         <v>1</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -945,11 +977,17 @@
       <c r="T4">
         <v>1</v>
       </c>
-      <c r="U4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1010,11 +1048,17 @@
       <c r="T5">
         <v>1</v>
       </c>
-      <c r="U5" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1075,11 +1119,17 @@
       <c r="T6">
         <v>1</v>
       </c>
-      <c r="U6" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1140,11 +1190,17 @@
       <c r="T7">
         <v>1</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1205,11 +1261,17 @@
       <c r="T8">
         <v>1</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1270,7 +1332,13 @@
       <c r="T9">
         <v>1</v>
       </c>
-      <c r="U9" s="9" t="s">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fill-in temporary SSD values
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB8AD16-6402-49EA-8211-B57215303034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEDBFE6-C8BE-45A8-8F80-B3E1FC656454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
@@ -233,7 +233,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="175" formatCode="#,##0.0000000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,14 +287,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -328,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,7 +335,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -677,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A82EF9-D59D-445F-8AC5-80173FC1E833}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,9 +694,11 @@
     <col min="16" max="16" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.44140625" style="5" customWidth="1"/>
-    <col min="20" max="20" width="10.21875" style="6" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="5"/>
+    <col min="19" max="19" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.77734375" style="5" customWidth="1"/>
+    <col min="22" max="22" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -829,17 +827,17 @@
       <c r="R2">
         <v>200</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="9">
-        <v>1</v>
+      <c r="S2" s="9">
+        <v>5.62403837498222</v>
+      </c>
+      <c r="T2" s="9">
+        <v>3.5474401150413999</v>
+      </c>
+      <c r="U2" s="10">
+        <v>4.5749362947466601</v>
+      </c>
+      <c r="V2" s="10">
+        <v>3.5763253838757199</v>
       </c>
       <c r="W2" t="s">
         <v>18</v>
@@ -900,17 +898,17 @@
       <c r="R3">
         <v>589</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
+      <c r="S3" s="9">
+        <v>6.3278947960519503</v>
+      </c>
+      <c r="T3" s="9">
+        <v>1.4072597346019999</v>
+      </c>
+      <c r="U3" s="10">
+        <v>4.3489598354767596</v>
+      </c>
+      <c r="V3" s="10">
+        <v>2.1585237091479801</v>
       </c>
       <c r="W3" t="s">
         <v>19</v>
@@ -971,17 +969,17 @@
       <c r="R4">
         <v>55.3</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>1</v>
+      <c r="S4" s="9">
+        <v>9.1061606298088602</v>
+      </c>
+      <c r="T4" s="9">
+        <v>2.6069120379527702</v>
+      </c>
+      <c r="U4" s="10">
+        <v>6.9981781628115796</v>
+      </c>
+      <c r="V4" s="10">
+        <v>2.0393695635427598</v>
       </c>
       <c r="W4" t="s">
         <v>20</v>
@@ -1042,17 +1040,17 @@
       <c r="R5">
         <v>59</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
+      <c r="S5" s="9">
+        <v>9.8905565953578805</v>
+      </c>
+      <c r="T5" s="9">
+        <v>2.7205387873979001</v>
+      </c>
+      <c r="U5" s="10">
+        <v>6.43679151778346</v>
+      </c>
+      <c r="V5" s="10">
+        <v>2.6401788533431398</v>
       </c>
       <c r="W5" s="5" t="s">
         <v>58</v>
@@ -1113,17 +1111,17 @@
       <c r="R6">
         <v>5247</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>1</v>
+      <c r="S6" s="9">
+        <v>7.6053726530939603</v>
+      </c>
+      <c r="T6" s="9">
+        <v>1.5097981215035301</v>
+      </c>
+      <c r="U6" s="10">
+        <v>4.0867019565803897</v>
+      </c>
+      <c r="V6" s="10">
+        <v>2.5027507539066902</v>
       </c>
       <c r="W6" s="5" t="s">
         <v>58</v>
@@ -1184,17 +1182,17 @@
       <c r="R7">
         <v>3200</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>1</v>
+      <c r="S7" s="9">
+        <v>5.4654907850452998</v>
+      </c>
+      <c r="T7" s="9">
+        <v>1.77917615897989</v>
+      </c>
+      <c r="U7" s="10">
+        <v>2.506282807162</v>
+      </c>
+      <c r="V7" s="10">
+        <v>2.1588197690050399</v>
       </c>
       <c r="W7" t="s">
         <v>23</v>
@@ -1255,17 +1253,17 @@
       <c r="R8">
         <v>73.88</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
+      <c r="S8" s="9">
+        <v>9.8633236942744809</v>
+      </c>
+      <c r="T8" s="9">
+        <v>2.8744929689301202</v>
+      </c>
+      <c r="U8" s="10">
+        <v>6.6031309598935701</v>
+      </c>
+      <c r="V8" s="10">
+        <v>2.9285198026244799</v>
       </c>
       <c r="W8" t="s">
         <v>24</v>
@@ -1326,17 +1324,17 @@
       <c r="R9">
         <v>73.2</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
+      <c r="S9" s="9">
+        <v>7.0701986255061797</v>
+      </c>
+      <c r="T9" s="9">
+        <v>3.6329701694213301</v>
+      </c>
+      <c r="U9" s="10">
+        <v>4.5035906008342703</v>
+      </c>
+      <c r="V9" s="10">
+        <v>3.2432571146546199</v>
       </c>
       <c r="W9" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Correct low-level risk computation helper
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEDBFE6-C8BE-45A8-8F80-B3E1FC656454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A11351-035F-4205-8C0E-52D0D5219F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>chemical</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t>tmoa</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>ssd_acute_mu</t>
@@ -234,7 +231,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -335,8 +332,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -674,7 +671,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:V9"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,16 +754,16 @@
         <v>56</v>
       </c>
       <c r="S1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="W1" s="8" t="s">
         <v>57</v>
@@ -833,10 +830,10 @@
       <c r="T2" s="9">
         <v>3.5474401150413999</v>
       </c>
-      <c r="U2" s="10">
+      <c r="U2" s="9">
         <v>4.5749362947466601</v>
       </c>
-      <c r="V2" s="10">
+      <c r="V2" s="9">
         <v>3.5763253838757199</v>
       </c>
       <c r="W2" t="s">
@@ -904,10 +901,10 @@
       <c r="T3" s="9">
         <v>1.4072597346019999</v>
       </c>
-      <c r="U3" s="10">
+      <c r="U3" s="9">
         <v>4.3489598354767596</v>
       </c>
-      <c r="V3" s="10">
+      <c r="V3" s="9">
         <v>2.1585237091479801</v>
       </c>
       <c r="W3" t="s">
@@ -975,10 +972,10 @@
       <c r="T4" s="9">
         <v>2.6069120379527702</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U4" s="9">
         <v>6.9981781628115796</v>
       </c>
-      <c r="V4" s="10">
+      <c r="V4" s="9">
         <v>2.0393695635427598</v>
       </c>
       <c r="W4" t="s">
@@ -1046,14 +1043,14 @@
       <c r="T5" s="9">
         <v>2.7205387873979001</v>
       </c>
-      <c r="U5" s="10">
+      <c r="U5" s="9">
         <v>6.43679151778346</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5" s="9">
         <v>2.6401788533431398</v>
       </c>
-      <c r="W5" s="5" t="s">
-        <v>58</v>
+      <c r="W5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -1117,14 +1114,14 @@
       <c r="T6" s="9">
         <v>1.5097981215035301</v>
       </c>
-      <c r="U6" s="10">
+      <c r="U6" s="9">
         <v>4.0867019565803897</v>
       </c>
-      <c r="V6" s="10">
+      <c r="V6" s="9">
         <v>2.5027507539066902</v>
       </c>
-      <c r="W6" s="5" t="s">
-        <v>58</v>
+      <c r="W6" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -1188,10 +1185,10 @@
       <c r="T7" s="9">
         <v>1.77917615897989</v>
       </c>
-      <c r="U7" s="10">
+      <c r="U7" s="9">
         <v>2.506282807162</v>
       </c>
-      <c r="V7" s="10">
+      <c r="V7" s="9">
         <v>2.1588197690050399</v>
       </c>
       <c r="W7" t="s">
@@ -1259,10 +1256,10 @@
       <c r="T8" s="9">
         <v>2.8744929689301202</v>
       </c>
-      <c r="U8" s="10">
+      <c r="U8" s="9">
         <v>6.6031309598935701</v>
       </c>
-      <c r="V8" s="10">
+      <c r="V8" s="9">
         <v>2.9285198026244799</v>
       </c>
       <c r="W8" t="s">
@@ -1330,10 +1327,10 @@
       <c r="T9" s="9">
         <v>3.6329701694213301</v>
       </c>
-      <c r="U9" s="10">
+      <c r="U9" s="9">
         <v>4.5035906008342703</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="9">
         <v>3.2432571146546199</v>
       </c>
       <c r="W9" t="s">

</xml_diff>

<commit_message>
Review pesticide names (close #333)
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A11351-035F-4205-8C0E-52D0D5219F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79767FE-D084-4A32-8688-BA4C102856CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
+    <workbookView xWindow="-28920" yWindow="-7230" windowWidth="29040" windowHeight="15720" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical Properties" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>chemical</t>
   </si>
@@ -224,6 +224,24 @@
   </si>
   <si>
     <t>ssd_chronic_sigma</t>
+  </si>
+  <si>
+    <t>Azoxystrobin</t>
+  </si>
+  <si>
+    <t>Bentazone</t>
+  </si>
+  <si>
+    <t>Cycloxydim</t>
+  </si>
+  <si>
+    <t>Cyhalofop-butyl</t>
+  </si>
+  <si>
+    <t>Difenoconazole</t>
+  </si>
+  <si>
+    <t>Penoxsulam</t>
   </si>
 </sst>
 </file>
@@ -670,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A82EF9-D59D-445F-8AC5-80173FC1E833}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
@@ -842,7 +860,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -908,12 +926,12 @@
         <v>2.1585237091479801</v>
       </c>
       <c r="W3" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -979,12 +997,12 @@
         <v>2.0393695635427598</v>
       </c>
       <c r="W4" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1050,12 +1068,12 @@
         <v>2.6401788533431398</v>
       </c>
       <c r="W5" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1121,12 +1139,12 @@
         <v>2.5027507539066902</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1192,7 +1210,7 @@
         <v>2.1588197690050399</v>
       </c>
       <c r="W7" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -1268,7 +1286,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1334,7 +1352,7 @@
         <v>3.2432571146546199</v>
       </c>
       <c r="W9" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix TMoAs names (close #372)
</commit_message>
<xml_diff>
--- a/data-raw/raw/ct_parameters.xlsx
+++ b/data-raw/raw/ct_parameters.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valerio\Code\erahumed\erahumed\data-raw\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79767FE-D084-4A32-8688-BA4C102856CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A38673D-F481-47E7-B372-A54718AB52AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-7230" windowWidth="29040" windowHeight="15720" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
+    <workbookView xWindow="-28920" yWindow="-6090" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1E4F0AD0-4D97-4600-9516-2EBF7D3724AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical Properties" sheetId="14" r:id="rId1"/>
-    <sheet name="Chemical Properties (OLD)" sheetId="13" r:id="rId2"/>
+    <sheet name="Toxic Modes of Action" sheetId="13" r:id="rId2"/>
     <sheet name="Global Properties" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>chemical</t>
   </si>
@@ -49,9 +49,6 @@
     <t>fet_cm</t>
   </si>
   <si>
-    <t>kd_cm3_g</t>
-  </si>
-  <si>
     <t>kf_day</t>
   </si>
   <si>
@@ -97,27 +94,9 @@
     <t>Acetamiprid</t>
   </si>
   <si>
-    <t>Azoxy</t>
-  </si>
-  <si>
-    <t>Benta</t>
-  </si>
-  <si>
-    <t>Cicloxidim</t>
-  </si>
-  <si>
-    <t>Cyhalo</t>
-  </si>
-  <si>
-    <t>Difeno</t>
-  </si>
-  <si>
     <t>MCPA</t>
   </si>
   <si>
-    <t>Penoxulam</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -211,9 +190,6 @@
     <t>koc_cm3_g</t>
   </si>
   <si>
-    <t>tmoa</t>
-  </si>
-  <si>
     <t>ssd_acute_mu</t>
   </si>
   <si>
@@ -242,6 +218,60 @@
   </si>
   <si>
     <t>Penoxsulam</t>
+  </si>
+  <si>
+    <t>C_Respiration</t>
+  </si>
+  <si>
+    <t>AcetylCoA</t>
+  </si>
+  <si>
+    <t>Photosynthesis_PSII</t>
+  </si>
+  <si>
+    <t>Sterol_biosynthesis</t>
+  </si>
+  <si>
+    <t>Auxin_mimics</t>
+  </si>
+  <si>
+    <t>AcetoLactate</t>
+  </si>
+  <si>
+    <t>NicotinicAcetylcholine</t>
+  </si>
+  <si>
+    <t>Nicotinic Acetylcholine Receptor Agonists</t>
+  </si>
+  <si>
+    <t>Cellular Respiration Inhibition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NicotinicAcetylcholine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AcetoLactate </t>
+  </si>
+  <si>
+    <t>Photosynthesis Inhibition at Photosystem II</t>
+  </si>
+  <si>
+    <t>Acetyl-CoA Carboxylase Inhibitors</t>
+  </si>
+  <si>
+    <t>Sterol Biosynthesis Inhibitors</t>
+  </si>
+  <si>
+    <t>Auxin Mimics</t>
+  </si>
+  <si>
+    <t>Inhibition of Acetolactate Synthase</t>
+  </si>
+  <si>
+    <t>tmoa_id</t>
+  </si>
+  <si>
+    <t>tmoa_name</t>
   </si>
 </sst>
 </file>
@@ -303,21 +333,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -325,33 +349,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -688,108 +698,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A82EF9-D59D-445F-8AC5-80173FC1E833}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView topLeftCell="I1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.44140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.44140625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.77734375" style="5" customWidth="1"/>
-    <col min="22" max="22" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.77734375" style="3" customWidth="1"/>
+    <col min="22" max="22" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>57</v>
+      <c r="R1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -842,25 +852,25 @@
       <c r="R2">
         <v>200</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="7">
         <v>5.62403837498222</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="7">
         <v>3.5474401150413999</v>
       </c>
-      <c r="U2" s="9">
+      <c r="U2" s="7">
         <v>4.5749362947466601</v>
       </c>
-      <c r="V2" s="9">
+      <c r="V2" s="7">
         <v>3.5763253838757199</v>
       </c>
       <c r="W2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -913,25 +923,25 @@
       <c r="R3">
         <v>589</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="7">
         <v>6.3278947960519503</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="7">
         <v>1.4072597346019999</v>
       </c>
-      <c r="U3" s="9">
+      <c r="U3" s="7">
         <v>4.3489598354767596</v>
       </c>
-      <c r="V3" s="9">
+      <c r="V3" s="7">
         <v>2.1585237091479801</v>
       </c>
       <c r="W3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -984,25 +994,25 @@
       <c r="R4">
         <v>55.3</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="7">
         <v>9.1061606298088602</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="7">
         <v>2.6069120379527702</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U4" s="7">
         <v>6.9981781628115796</v>
       </c>
-      <c r="V4" s="9">
+      <c r="V4" s="7">
         <v>2.0393695635427598</v>
       </c>
       <c r="W4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1055,25 +1065,25 @@
       <c r="R5">
         <v>59</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="7">
         <v>9.8905565953578805</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="7">
         <v>2.7205387873979001</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="7">
         <v>6.43679151778346</v>
       </c>
-      <c r="V5" s="9">
+      <c r="V5" s="7">
         <v>2.6401788533431398</v>
       </c>
       <c r="W5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1126,25 +1136,25 @@
       <c r="R6">
         <v>5247</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="7">
         <v>7.6053726530939603</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="7">
         <v>1.5097981215035301</v>
       </c>
-      <c r="U6" s="9">
+      <c r="U6" s="7">
         <v>4.0867019565803897</v>
       </c>
-      <c r="V6" s="9">
+      <c r="V6" s="7">
         <v>2.5027507539066902</v>
       </c>
-      <c r="W6" s="10" t="s">
-        <v>64</v>
+      <c r="W6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1197,25 +1207,25 @@
       <c r="R7">
         <v>3200</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="7">
         <v>5.4654907850452998</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="7">
         <v>1.77917615897989</v>
       </c>
-      <c r="U7" s="9">
+      <c r="U7" s="7">
         <v>2.506282807162</v>
       </c>
-      <c r="V7" s="9">
+      <c r="V7" s="7">
         <v>2.1588197690050399</v>
       </c>
       <c r="W7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1268,25 +1278,25 @@
       <c r="R8">
         <v>73.88</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="7">
         <v>9.8633236942744809</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="7">
         <v>2.8744929689301202</v>
       </c>
-      <c r="U8" s="9">
+      <c r="U8" s="7">
         <v>6.6031309598935701</v>
       </c>
-      <c r="V8" s="9">
+      <c r="V8" s="7">
         <v>2.9285198026244799</v>
       </c>
       <c r="W8" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1339,20 +1349,20 @@
       <c r="R9">
         <v>73.2</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="7">
         <v>7.0701986255061797</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="7">
         <v>3.6329701694213301</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U9" s="7">
         <v>4.5035906008342703</v>
       </c>
-      <c r="V9" s="9">
+      <c r="V9" s="7">
         <v>3.2432571146546199</v>
       </c>
       <c r="W9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1363,521 +1373,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB6CF40-947E-4F43-9725-E413236A1838}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="18" width="7.44140625" customWidth="1"/>
     <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0.2</v>
-      </c>
-      <c r="D2">
-        <v>5.8</v>
-      </c>
-      <c r="E2">
-        <v>0.11002336199364211</v>
-      </c>
-      <c r="F2">
-        <v>0.23104906018664842</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <v>0.23104906018664842</v>
-      </c>
-      <c r="I2">
-        <v>20</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>3.5185136069032757E-2</v>
-      </c>
-      <c r="M2">
-        <v>20</v>
-      </c>
-      <c r="N2">
-        <v>222.67699999999999</v>
-      </c>
-      <c r="O2">
-        <v>2.58</v>
-      </c>
-      <c r="P2">
-        <v>2.58</v>
-      </c>
-      <c r="Q2">
-        <v>2.58</v>
-      </c>
-      <c r="R2">
-        <v>2950</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0.2</v>
-      </c>
-      <c r="D3">
-        <v>208.22</v>
-      </c>
-      <c r="E3">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="F3">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I3">
-        <v>20</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L3">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="M3">
-        <v>20</v>
-      </c>
-      <c r="N3">
-        <v>403.33800000000002</v>
-      </c>
-      <c r="O3">
-        <v>2.6</v>
-      </c>
-      <c r="P3">
-        <v>2.6</v>
-      </c>
-      <c r="Q3">
-        <v>2.6</v>
-      </c>
-      <c r="R3">
-        <v>6.73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0.2</v>
-      </c>
-      <c r="D4">
-        <v>1.6</v>
-      </c>
-      <c r="E4">
-        <v>0.46200000000000002</v>
-      </c>
-      <c r="F4">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-      <c r="H4">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="I4">
-        <v>20</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>0.01</v>
-      </c>
-      <c r="L4">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="M4">
-        <v>20</v>
-      </c>
-      <c r="N4">
-        <v>240.28</v>
-      </c>
-      <c r="O4">
-        <v>2.58</v>
-      </c>
-      <c r="P4">
-        <v>2.58</v>
-      </c>
-      <c r="Q4">
-        <v>2.58</v>
-      </c>
-      <c r="R4">
-        <v>7112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0.2</v>
-      </c>
-      <c r="D5">
-        <v>2.1</v>
-      </c>
-      <c r="E5">
-        <v>0.24755256448569476</v>
-      </c>
-      <c r="F5">
-        <v>3.0136833937388925E-2</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
-        <v>0.11748257297626191</v>
-      </c>
-      <c r="I5">
-        <v>20</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>4.6209812037329684E-2</v>
-      </c>
-      <c r="M5">
-        <v>20</v>
-      </c>
-      <c r="N5">
-        <v>325.5</v>
-      </c>
-      <c r="O5">
-        <v>2.6</v>
-      </c>
-      <c r="P5">
-        <v>2.6</v>
-      </c>
-      <c r="Q5">
-        <v>2.6</v>
-      </c>
-      <c r="R5">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0.2</v>
-      </c>
-      <c r="D6">
-        <v>5.39</v>
-      </c>
-      <c r="E6">
-        <v>0.161</v>
-      </c>
-      <c r="F6">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I6">
-        <v>20</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0.126</v>
-      </c>
-      <c r="M6">
-        <v>20</v>
-      </c>
-      <c r="N6">
-        <v>357.38</v>
-      </c>
-      <c r="O6">
-        <v>2.58</v>
-      </c>
-      <c r="P6">
-        <v>2.58</v>
-      </c>
-      <c r="Q6">
-        <v>2.58</v>
-      </c>
-      <c r="R6">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0.2</v>
-      </c>
-      <c r="D7">
-        <v>109.04</v>
-      </c>
-      <c r="E7">
-        <v>9.4E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
-      </c>
-      <c r="H7">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I7">
-        <v>20</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7">
-        <v>1E-3</v>
-      </c>
-      <c r="L7">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="M7">
-        <v>20</v>
-      </c>
-      <c r="N7">
-        <v>406.3</v>
-      </c>
-      <c r="O7">
-        <v>2.6</v>
-      </c>
-      <c r="P7">
-        <v>2.6</v>
-      </c>
-      <c r="Q7">
-        <v>2.6</v>
-      </c>
-      <c r="R7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0.2</v>
-      </c>
-      <c r="D8">
-        <v>0.03</v>
-      </c>
-      <c r="E8">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="F8">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
-      <c r="H8">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="I8">
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="M8">
-        <v>20</v>
-      </c>
-      <c r="N8">
-        <v>200.62</v>
-      </c>
-      <c r="O8">
-        <v>2.58</v>
-      </c>
-      <c r="P8">
-        <v>2.58</v>
-      </c>
-      <c r="Q8">
-        <v>2.58</v>
-      </c>
-      <c r="R8">
-        <v>29390</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0.2</v>
-      </c>
-      <c r="D9">
-        <v>2.1</v>
-      </c>
-      <c r="E9">
-        <v>0.248</v>
-      </c>
-      <c r="F9">
-        <v>0.03</v>
-      </c>
-      <c r="G9">
-        <v>20</v>
-      </c>
-      <c r="H9">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="I9">
-        <v>20</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="M9">
-        <v>20</v>
-      </c>
-      <c r="N9">
-        <v>483.4</v>
-      </c>
-      <c r="O9">
-        <v>2.58</v>
-      </c>
-      <c r="P9">
-        <v>2.58</v>
-      </c>
-      <c r="Q9">
-        <v>2.58</v>
-      </c>
-      <c r="R9">
-        <v>408</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1902,170 +1472,170 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>0.5</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>0.24</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>0.35</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C6">
         <v>1.5</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>